<commit_message>
update to tower height curve
</commit_message>
<xml_diff>
--- a/gen3_project_files/resource/tower-height-power.xlsx
+++ b/gen3_project_files/resource/tower-height-power.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mwagner\Documents\NREL\repositories\ssc-gen3\gen3_project_files\resource\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4DA65A5-D012-489E-AC95-41C1511276AC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D551DA4-FD0D-4771-9898-DC6CDA23B522}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E882345E-7BFC-4D39-BA33-82B992290FF8}"/>
+    <workbookView xWindow="3030" yWindow="3030" windowWidth="21600" windowHeight="11385" xr2:uid="{E882345E-7BFC-4D39-BA33-82B992290FF8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -626,7 +626,13 @@
             <c:dispRSqr val="0"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.17522912095004517"/>
+                  <c:y val="0.60781464670487162"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="0.0000E+00" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
                 <a:ln>

</xml_diff>